<commit_message>
Update sample opendata_covid19_naracity.xlsx, add death_count
</commit_message>
<xml_diff>
--- a/sample/opendata_covid19_NaraCity.xlsx
+++ b/sample/opendata_covid19_NaraCity.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Js-fil001\共有\000010共通フォルダ\(1)保険予防課・医療政策課→秘書広報課\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasushi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4837E42-F94F-4DC3-BBDE-8156705AA327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52860" yWindow="495" windowWidth="24435" windowHeight="18990" tabRatio="775" activeTab="1"/>
+    <workbookView xWindow="60960" yWindow="5790" windowWidth="20565" windowHeight="13890" tabRatio="775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.陽性患者リスト" sheetId="8" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="陽性患者リストの定義" sheetId="14" r:id="rId4"/>
     <sheet name="感染症状況の定義" sheetId="15" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataSignature="AMtx7mjH4chSrTCU+u+bcA2KRSGrmpOPZA=="/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="142">
   <si>
     <t>・本データ項目定義書は、新型コロナウイルス感染症対策の一環として、各自治体において標準フォーマットでのオープンデータを公開できるように支援するためのものです</t>
   </si>
@@ -1016,11 +1017,24 @@
     </rPh>
     <phoneticPr fontId="4"/>
   </si>
+  <si>
+    <t>死亡者数_累計</t>
+    <rPh sb="0" eb="3">
+      <t>シボウシャ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>スウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ルイケイ</t>
+    </rPh>
+    <phoneticPr fontId="14"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
@@ -1717,22 +1731,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="2" max="2" width="7.6171875" customWidth="1"/>
     <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.75" style="34" customWidth="1"/>
-    <col min="6" max="6" width="13.25" style="34" customWidth="1"/>
-    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="10.75" customWidth="1"/>
+    <col min="5" max="5" width="11.76171875" style="34" customWidth="1"/>
+    <col min="6" max="6" width="13.234375" style="34" customWidth="1"/>
+    <col min="7" max="7" width="9.76171875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.234375" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="10.76171875" customWidth="1"/>
     <col min="15" max="15" width="12" style="43" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3180,29 +3194,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="44" customWidth="1"/>
-    <col min="2" max="2" width="8.875" style="35" customWidth="1"/>
-    <col min="3" max="3" width="11.625" style="35" customWidth="1"/>
-    <col min="4" max="4" width="12.375" style="35" customWidth="1"/>
+    <col min="1" max="1" width="13.37890625" style="44" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="35" customWidth="1"/>
+    <col min="3" max="3" width="11.6171875" style="35" customWidth="1"/>
+    <col min="4" max="4" width="12.37890625" style="35" customWidth="1"/>
     <col min="5" max="5" width="13" style="39" customWidth="1"/>
-    <col min="6" max="8" width="11.375" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.125" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.125" style="35" customWidth="1"/>
-    <col min="12" max="12" width="17" style="35" customWidth="1"/>
-    <col min="13" max="16384" width="8.75" style="35"/>
+    <col min="6" max="8" width="11.37890625" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" style="35" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" style="35" customWidth="1"/>
+    <col min="13" max="13" width="17" style="35" customWidth="1"/>
+    <col min="14" max="16384" width="8.76171875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="33.75">
+    <row r="1" spans="1:13" ht="31.5">
       <c r="A1" s="57" t="s">
         <v>95</v>
       </c>
@@ -3233,14 +3248,17 @@
       <c r="J1" s="63" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="K1" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="L1" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="62" t="s">
+      <c r="M1" s="62" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13" ht="14.1">
       <c r="A2" s="53">
         <v>43891</v>
       </c>
@@ -3257,16 +3275,19 @@
       <c r="F2" s="55">
         <v>0</v>
       </c>
-      <c r="G2" s="52"/>
+      <c r="G2" s="52">
+        <v>0</v>
+      </c>
       <c r="H2" s="52"/>
       <c r="I2" s="56"/>
       <c r="J2" s="56"/>
-      <c r="K2" s="52">
+      <c r="K2" s="56"/>
+      <c r="L2" s="52">
         <v>23</v>
       </c>
-      <c r="L2" s="52"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="52"/>
+    </row>
+    <row r="3" spans="1:13" ht="14.1">
       <c r="A3" s="53">
         <v>43892</v>
       </c>
@@ -3283,16 +3304,19 @@
       <c r="F3" s="55">
         <v>3</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="52">
+        <v>0</v>
+      </c>
       <c r="H3" s="52"/>
       <c r="I3" s="56"/>
       <c r="J3" s="56"/>
-      <c r="K3" s="52">
+      <c r="K3" s="56"/>
+      <c r="L3" s="52">
         <v>57</v>
       </c>
-      <c r="L3" s="52"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="52"/>
+    </row>
+    <row r="4" spans="1:13" ht="14.1">
       <c r="A4" s="53">
         <v>43893</v>
       </c>
@@ -3309,16 +3333,19 @@
       <c r="F4" s="55">
         <v>1</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="52">
+        <v>0</v>
+      </c>
       <c r="H4" s="52"/>
       <c r="I4" s="56"/>
       <c r="J4" s="56"/>
-      <c r="K4" s="52">
+      <c r="K4" s="56"/>
+      <c r="L4" s="52">
         <v>54</v>
       </c>
-      <c r="L4" s="52"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="52"/>
+    </row>
+    <row r="5" spans="1:13" ht="14.1">
       <c r="A5" s="53">
         <v>43894</v>
       </c>
@@ -3335,16 +3362,19 @@
       <c r="F5" s="55">
         <v>3</v>
       </c>
-      <c r="G5" s="52"/>
+      <c r="G5" s="52">
+        <v>0</v>
+      </c>
       <c r="H5" s="52"/>
       <c r="I5" s="56"/>
       <c r="J5" s="56"/>
-      <c r="K5" s="52">
+      <c r="K5" s="56"/>
+      <c r="L5" s="52">
         <v>45</v>
       </c>
-      <c r="L5" s="52"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="52"/>
+    </row>
+    <row r="6" spans="1:13" ht="14.1">
       <c r="A6" s="53">
         <v>43895</v>
       </c>
@@ -3361,16 +3391,19 @@
       <c r="F6" s="55">
         <v>5</v>
       </c>
-      <c r="G6" s="52"/>
+      <c r="G6" s="52">
+        <v>0</v>
+      </c>
       <c r="H6" s="52"/>
       <c r="I6" s="56"/>
       <c r="J6" s="56"/>
-      <c r="K6" s="52">
+      <c r="K6" s="56"/>
+      <c r="L6" s="52">
         <v>62</v>
       </c>
-      <c r="L6" s="52"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="52"/>
+    </row>
+    <row r="7" spans="1:13" ht="14.1">
       <c r="A7" s="53">
         <v>43896</v>
       </c>
@@ -3393,12 +3426,13 @@
       <c r="H7" s="52"/>
       <c r="I7" s="56"/>
       <c r="J7" s="56"/>
-      <c r="K7" s="52">
+      <c r="K7" s="56"/>
+      <c r="L7" s="52">
         <v>50</v>
       </c>
-      <c r="L7" s="52"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="52"/>
+    </row>
+    <row r="8" spans="1:13" ht="14.1">
       <c r="A8" s="53">
         <v>43897</v>
       </c>
@@ -3415,15 +3449,19 @@
       <c r="F8" s="55">
         <v>2</v>
       </c>
+      <c r="G8" s="35">
+        <v>0</v>
+      </c>
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>
       <c r="J8" s="56"/>
-      <c r="K8" s="52">
+      <c r="K8" s="56"/>
+      <c r="L8" s="52">
         <v>38</v>
       </c>
-      <c r="L8" s="52"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="52"/>
+    </row>
+    <row r="9" spans="1:13" ht="14.1">
       <c r="A9" s="53">
         <v>43898</v>
       </c>
@@ -3440,15 +3478,19 @@
       <c r="F9" s="55">
         <v>3</v>
       </c>
+      <c r="G9" s="35">
+        <v>0</v>
+      </c>
       <c r="H9" s="52"/>
       <c r="I9" s="56"/>
       <c r="J9" s="56"/>
-      <c r="K9" s="52">
+      <c r="K9" s="56"/>
+      <c r="L9" s="52">
         <v>30</v>
       </c>
-      <c r="L9" s="52"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" s="52"/>
+    </row>
+    <row r="10" spans="1:13" ht="14.1">
       <c r="A10" s="53">
         <v>43899</v>
       </c>
@@ -3465,15 +3507,19 @@
       <c r="F10" s="55">
         <v>2</v>
       </c>
+      <c r="G10" s="35">
+        <v>0</v>
+      </c>
       <c r="H10" s="52"/>
       <c r="I10" s="56"/>
       <c r="J10" s="56"/>
-      <c r="K10" s="52">
+      <c r="K10" s="56"/>
+      <c r="L10" s="52">
         <v>88</v>
       </c>
-      <c r="L10" s="52"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="52"/>
+    </row>
+    <row r="11" spans="1:13" ht="14.1">
       <c r="A11" s="53">
         <v>43900</v>
       </c>
@@ -3490,15 +3536,19 @@
       <c r="F11" s="55">
         <v>7</v>
       </c>
+      <c r="G11" s="35">
+        <v>0</v>
+      </c>
       <c r="H11" s="52"/>
       <c r="I11" s="56"/>
       <c r="J11" s="56"/>
-      <c r="K11" s="52">
+      <c r="K11" s="56"/>
+      <c r="L11" s="52">
         <v>67</v>
       </c>
-      <c r="L11" s="52"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" s="52"/>
+    </row>
+    <row r="12" spans="1:13" ht="14.1">
       <c r="A12" s="53">
         <v>43901</v>
       </c>
@@ -3521,12 +3571,13 @@
       <c r="H12" s="52"/>
       <c r="I12" s="56"/>
       <c r="J12" s="56"/>
-      <c r="K12" s="52">
+      <c r="K12" s="56"/>
+      <c r="L12" s="52">
         <v>52</v>
       </c>
-      <c r="L12" s="52"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" s="52"/>
+    </row>
+    <row r="13" spans="1:13" ht="14.1">
       <c r="A13" s="53">
         <v>43902</v>
       </c>
@@ -3543,15 +3594,19 @@
       <c r="F13" s="55">
         <v>0</v>
       </c>
+      <c r="G13" s="35">
+        <v>0</v>
+      </c>
       <c r="H13" s="52"/>
       <c r="I13" s="56"/>
       <c r="J13" s="56"/>
-      <c r="K13" s="52">
+      <c r="K13" s="56"/>
+      <c r="L13" s="52">
         <v>60</v>
       </c>
-      <c r="L13" s="52"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" s="52"/>
+    </row>
+    <row r="14" spans="1:13" ht="14.1">
       <c r="A14" s="53">
         <v>43903</v>
       </c>
@@ -3568,15 +3623,19 @@
       <c r="F14" s="55">
         <v>3</v>
       </c>
+      <c r="G14" s="35">
+        <v>0</v>
+      </c>
       <c r="H14" s="52"/>
       <c r="I14" s="56"/>
       <c r="J14" s="56"/>
-      <c r="K14" s="52">
+      <c r="K14" s="56"/>
+      <c r="L14" s="52">
         <v>59</v>
       </c>
-      <c r="L14" s="52"/>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" s="52"/>
+    </row>
+    <row r="15" spans="1:13" ht="14.1">
       <c r="A15" s="53">
         <v>43904</v>
       </c>
@@ -3593,15 +3652,19 @@
       <c r="F15" s="55">
         <v>3</v>
       </c>
+      <c r="G15" s="35">
+        <v>0</v>
+      </c>
       <c r="H15" s="52"/>
       <c r="I15" s="56"/>
       <c r="J15" s="56"/>
-      <c r="K15" s="52">
+      <c r="K15" s="56"/>
+      <c r="L15" s="52">
         <v>33</v>
       </c>
-      <c r="L15" s="52"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" s="52"/>
+    </row>
+    <row r="16" spans="1:13" ht="14.1">
       <c r="A16" s="53">
         <v>43905</v>
       </c>
@@ -3618,15 +3681,19 @@
       <c r="F16" s="55">
         <v>2</v>
       </c>
+      <c r="G16" s="35">
+        <v>0</v>
+      </c>
       <c r="H16" s="52"/>
       <c r="I16" s="56"/>
       <c r="J16" s="56"/>
-      <c r="K16" s="52">
+      <c r="K16" s="56"/>
+      <c r="L16" s="52">
         <v>21</v>
       </c>
-      <c r="L16" s="52"/>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="52"/>
+    </row>
+    <row r="17" spans="1:13" ht="14.1">
       <c r="A17" s="53">
         <v>43906</v>
       </c>
@@ -3643,15 +3710,19 @@
       <c r="F17" s="55">
         <v>0</v>
       </c>
+      <c r="G17" s="35">
+        <v>0</v>
+      </c>
       <c r="H17" s="52"/>
       <c r="I17" s="56"/>
       <c r="J17" s="56"/>
-      <c r="K17" s="52">
+      <c r="K17" s="56"/>
+      <c r="L17" s="52">
         <v>82</v>
       </c>
-      <c r="L17" s="52"/>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="52"/>
+    </row>
+    <row r="18" spans="1:13" ht="14.1">
       <c r="A18" s="53">
         <v>43907</v>
       </c>
@@ -3668,15 +3739,19 @@
       <c r="F18" s="55">
         <v>5</v>
       </c>
+      <c r="G18" s="35">
+        <v>0</v>
+      </c>
       <c r="H18" s="52"/>
       <c r="I18" s="56"/>
       <c r="J18" s="56"/>
-      <c r="K18" s="52">
+      <c r="K18" s="56"/>
+      <c r="L18" s="52">
         <v>34</v>
       </c>
-      <c r="L18" s="52"/>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="52"/>
+    </row>
+    <row r="19" spans="1:13" ht="14.1">
       <c r="A19" s="53">
         <v>43908</v>
       </c>
@@ -3693,15 +3768,19 @@
       <c r="F19" s="55">
         <v>3</v>
       </c>
+      <c r="G19" s="35">
+        <v>0</v>
+      </c>
       <c r="H19" s="52"/>
       <c r="I19" s="56"/>
       <c r="J19" s="56"/>
-      <c r="K19" s="52">
+      <c r="K19" s="56"/>
+      <c r="L19" s="52">
         <v>60</v>
       </c>
-      <c r="L19" s="52"/>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="52"/>
+    </row>
+    <row r="20" spans="1:13" ht="14.1">
       <c r="A20" s="53">
         <v>43909</v>
       </c>
@@ -3718,15 +3797,19 @@
       <c r="F20" s="55">
         <v>6</v>
       </c>
+      <c r="G20" s="35">
+        <v>0</v>
+      </c>
       <c r="H20" s="52"/>
       <c r="I20" s="56"/>
       <c r="J20" s="56"/>
-      <c r="K20" s="52">
+      <c r="K20" s="56"/>
+      <c r="L20" s="52">
         <v>56</v>
       </c>
-      <c r="L20" s="52"/>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" s="52"/>
+    </row>
+    <row r="21" spans="1:13" ht="14.1">
       <c r="A21" s="53">
         <v>43910</v>
       </c>
@@ -3743,15 +3826,19 @@
       <c r="F21" s="55">
         <v>5</v>
       </c>
+      <c r="G21" s="35">
+        <v>0</v>
+      </c>
       <c r="H21" s="52"/>
       <c r="I21" s="56"/>
       <c r="J21" s="56"/>
-      <c r="K21" s="52">
+      <c r="K21" s="56"/>
+      <c r="L21" s="52">
         <v>23</v>
       </c>
-      <c r="L21" s="52"/>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="52"/>
+    </row>
+    <row r="22" spans="1:13" ht="14.1">
       <c r="A22" s="53">
         <v>43911</v>
       </c>
@@ -3768,15 +3855,19 @@
       <c r="F22" s="55">
         <v>3</v>
       </c>
+      <c r="G22" s="35">
+        <v>0</v>
+      </c>
       <c r="H22" s="52"/>
       <c r="I22" s="56"/>
       <c r="J22" s="56"/>
-      <c r="K22" s="52">
+      <c r="K22" s="56"/>
+      <c r="L22" s="52">
         <v>22</v>
       </c>
-      <c r="L22" s="52"/>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="52"/>
+    </row>
+    <row r="23" spans="1:13" ht="14.1">
       <c r="A23" s="53">
         <v>43912</v>
       </c>
@@ -3793,15 +3884,19 @@
       <c r="F23" s="55">
         <v>4</v>
       </c>
+      <c r="G23" s="35">
+        <v>0</v>
+      </c>
       <c r="H23" s="52"/>
       <c r="I23" s="56"/>
       <c r="J23" s="56"/>
-      <c r="K23" s="52">
+      <c r="K23" s="56"/>
+      <c r="L23" s="52">
         <v>30</v>
       </c>
-      <c r="L23" s="52"/>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="M23" s="52"/>
+    </row>
+    <row r="24" spans="1:13" ht="14.1">
       <c r="A24" s="53">
         <v>43913</v>
       </c>
@@ -3818,15 +3913,19 @@
       <c r="F24" s="55">
         <v>1</v>
       </c>
+      <c r="G24" s="35">
+        <v>0</v>
+      </c>
       <c r="H24" s="52"/>
       <c r="I24" s="56"/>
       <c r="J24" s="56"/>
-      <c r="K24" s="52">
+      <c r="K24" s="56"/>
+      <c r="L24" s="52">
         <v>58</v>
       </c>
-      <c r="L24" s="52"/>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" s="52"/>
+    </row>
+    <row r="25" spans="1:13" ht="14.1">
       <c r="A25" s="53">
         <v>43914</v>
       </c>
@@ -3843,15 +3942,19 @@
       <c r="F25" s="55">
         <v>5</v>
       </c>
+      <c r="G25" s="35">
+        <v>0</v>
+      </c>
       <c r="H25" s="52"/>
       <c r="I25" s="56"/>
       <c r="J25" s="56"/>
-      <c r="K25" s="52">
+      <c r="K25" s="56"/>
+      <c r="L25" s="52">
         <v>32</v>
       </c>
-      <c r="L25" s="52"/>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="52"/>
+    </row>
+    <row r="26" spans="1:13" ht="14.1">
       <c r="A26" s="53">
         <v>43915</v>
       </c>
@@ -3868,15 +3971,19 @@
       <c r="F26" s="55">
         <v>3</v>
       </c>
+      <c r="G26" s="35">
+        <v>0</v>
+      </c>
       <c r="H26" s="52"/>
       <c r="I26" s="56"/>
       <c r="J26" s="56"/>
-      <c r="K26" s="52">
+      <c r="K26" s="56"/>
+      <c r="L26" s="52">
         <v>58</v>
       </c>
-      <c r="L26" s="52"/>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="M26" s="52"/>
+    </row>
+    <row r="27" spans="1:13" ht="14.1">
       <c r="A27" s="53">
         <v>43916</v>
       </c>
@@ -3893,15 +4000,19 @@
       <c r="F27" s="55">
         <v>10</v>
       </c>
+      <c r="G27" s="35">
+        <v>0</v>
+      </c>
       <c r="H27" s="52"/>
       <c r="I27" s="56"/>
       <c r="J27" s="56"/>
-      <c r="K27" s="52">
+      <c r="K27" s="56"/>
+      <c r="L27" s="52">
         <v>44</v>
       </c>
-      <c r="L27" s="52"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="M27" s="52"/>
+    </row>
+    <row r="28" spans="1:13" ht="14.1">
       <c r="A28" s="53">
         <v>43917</v>
       </c>
@@ -3918,15 +4029,19 @@
       <c r="F28" s="55">
         <v>3</v>
       </c>
+      <c r="G28" s="35">
+        <v>0</v>
+      </c>
       <c r="H28" s="52"/>
       <c r="I28" s="56"/>
       <c r="J28" s="56"/>
-      <c r="K28" s="52">
+      <c r="K28" s="56"/>
+      <c r="L28" s="52">
         <v>92</v>
       </c>
-      <c r="L28" s="52"/>
-    </row>
-    <row r="29" spans="1:12">
+      <c r="M28" s="52"/>
+    </row>
+    <row r="29" spans="1:13" ht="14.1">
       <c r="A29" s="53">
         <v>43918</v>
       </c>
@@ -3943,15 +4058,19 @@
       <c r="F29" s="55">
         <v>4</v>
       </c>
+      <c r="G29" s="35">
+        <v>0</v>
+      </c>
       <c r="H29" s="52"/>
       <c r="I29" s="56"/>
       <c r="J29" s="56"/>
-      <c r="K29" s="52">
+      <c r="K29" s="56"/>
+      <c r="L29" s="52">
         <v>62</v>
       </c>
-      <c r="L29" s="52"/>
-    </row>
-    <row r="30" spans="1:12">
+      <c r="M29" s="52"/>
+    </row>
+    <row r="30" spans="1:13" ht="14.1">
       <c r="A30" s="53">
         <v>43919</v>
       </c>
@@ -3968,15 +4087,19 @@
       <c r="F30" s="55">
         <v>0</v>
       </c>
+      <c r="G30" s="35">
+        <v>0</v>
+      </c>
       <c r="H30" s="52"/>
       <c r="I30" s="56"/>
       <c r="J30" s="56"/>
-      <c r="K30" s="52">
+      <c r="K30" s="56"/>
+      <c r="L30" s="52">
         <v>45</v>
       </c>
-      <c r="L30" s="52"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="M30" s="52"/>
+    </row>
+    <row r="31" spans="1:13" ht="14.1">
       <c r="A31" s="53">
         <v>43920</v>
       </c>
@@ -3993,15 +4116,19 @@
       <c r="F31" s="55">
         <v>1</v>
       </c>
+      <c r="G31" s="35">
+        <v>0</v>
+      </c>
       <c r="H31" s="52"/>
       <c r="I31" s="56"/>
       <c r="J31" s="56"/>
-      <c r="K31" s="52">
+      <c r="K31" s="56"/>
+      <c r="L31" s="52">
         <v>135</v>
       </c>
-      <c r="L31" s="52"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="M31" s="52"/>
+    </row>
+    <row r="32" spans="1:13" ht="14.1">
       <c r="A32" s="53">
         <v>43921</v>
       </c>
@@ -4018,15 +4145,19 @@
       <c r="F32" s="55">
         <v>1</v>
       </c>
+      <c r="G32" s="35">
+        <v>0</v>
+      </c>
       <c r="H32" s="52"/>
       <c r="I32" s="56"/>
       <c r="J32" s="56"/>
-      <c r="K32" s="52">
+      <c r="K32" s="56"/>
+      <c r="L32" s="52">
         <v>115</v>
       </c>
-      <c r="L32" s="52"/>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="M32" s="52"/>
+    </row>
+    <row r="33" spans="1:13" ht="14.1">
       <c r="A33" s="53">
         <v>43922</v>
       </c>
@@ -4046,12 +4177,12 @@
       <c r="G33" s="35">
         <v>1</v>
       </c>
-      <c r="K33" s="35">
+      <c r="L33" s="35">
         <v>142</v>
       </c>
-      <c r="L33" s="37"/>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="M33" s="37"/>
+    </row>
+    <row r="34" spans="1:13" ht="14.1">
       <c r="A34" s="53">
         <v>43923</v>
       </c>
@@ -4067,11 +4198,14 @@
       <c r="F34" s="35">
         <v>3</v>
       </c>
-      <c r="K34" s="35">
+      <c r="G34" s="35">
+        <v>0</v>
+      </c>
+      <c r="L34" s="35">
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:13" ht="14.1">
       <c r="A35" s="53">
         <v>43924</v>
       </c>
@@ -4087,11 +4221,14 @@
       <c r="F35" s="35">
         <v>5</v>
       </c>
-      <c r="K35" s="35">
+      <c r="G35" s="35">
+        <v>0</v>
+      </c>
+      <c r="L35" s="35">
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:13" ht="14.1">
       <c r="A36" s="53">
         <v>43925</v>
       </c>
@@ -4107,11 +4244,14 @@
       <c r="F36" s="35">
         <v>6</v>
       </c>
-      <c r="K36" s="35">
+      <c r="G36" s="35">
+        <v>0</v>
+      </c>
+      <c r="L36" s="35">
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:13" ht="14.1">
       <c r="A37" s="53">
         <v>43926</v>
       </c>
@@ -4127,11 +4267,14 @@
       <c r="F37" s="35">
         <v>2</v>
       </c>
-      <c r="K37" s="35">
+      <c r="G37" s="35">
+        <v>0</v>
+      </c>
+      <c r="L37" s="35">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:13" ht="14.1">
       <c r="A38" s="53">
         <v>43927</v>
       </c>
@@ -4150,11 +4293,11 @@
       <c r="G38" s="35">
         <v>1</v>
       </c>
-      <c r="K38" s="35">
+      <c r="L38" s="35">
         <v>211</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:13" ht="14.1">
       <c r="A39" s="53">
         <v>43928</v>
       </c>
@@ -4173,11 +4316,11 @@
       <c r="G39" s="35">
         <v>1</v>
       </c>
-      <c r="K39" s="35">
+      <c r="L39" s="35">
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:13" ht="14.1">
       <c r="A40" s="53">
         <v>43929</v>
       </c>
@@ -4193,12 +4336,14 @@
       <c r="F40" s="35">
         <v>0</v>
       </c>
-      <c r="G40" s="66"/>
-      <c r="K40" s="35">
+      <c r="G40" s="66">
+        <v>0</v>
+      </c>
+      <c r="L40" s="35">
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:13" ht="14.1">
       <c r="A41" s="53">
         <v>43930</v>
       </c>
@@ -4217,11 +4362,11 @@
       <c r="G41" s="66">
         <v>2</v>
       </c>
-      <c r="K41" s="35">
+      <c r="L41" s="35">
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:13" ht="14.1">
       <c r="A42" s="53">
         <v>43931</v>
       </c>
@@ -4240,11 +4385,11 @@
       <c r="G42" s="66">
         <v>1</v>
       </c>
-      <c r="K42" s="35">
+      <c r="L42" s="35">
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:13" ht="14.1">
       <c r="A43" s="53">
         <v>43932</v>
       </c>
@@ -4260,12 +4405,14 @@
       <c r="F43" s="35">
         <v>10</v>
       </c>
-      <c r="G43" s="66"/>
-      <c r="K43" s="35">
+      <c r="G43" s="66">
+        <v>0</v>
+      </c>
+      <c r="L43" s="35">
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:13" ht="14.1">
       <c r="A44" s="53">
         <v>43933</v>
       </c>
@@ -4281,8 +4428,19 @@
       <c r="F44" s="35">
         <v>4</v>
       </c>
-      <c r="G44" s="66"/>
+      <c r="G44" s="66">
+        <v>0</v>
+      </c>
+      <c r="I44" s="35">
+        <v>7</v>
+      </c>
+      <c r="J44" s="35">
+        <v>4</v>
+      </c>
       <c r="K44" s="35">
+        <v>1</v>
+      </c>
+      <c r="L44" s="35">
         <v>110</v>
       </c>
     </row>
@@ -4294,23 +4452,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E999"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="12.9"/>
   <cols>
-    <col min="1" max="1" width="13.125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="21.625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="50.125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="58.375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="5" customWidth="1"/>
-    <col min="7" max="26" width="9.375" style="5" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="5"/>
+    <col min="1" max="1" width="13.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="21.6171875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="50.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="58.37890625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="9.47265625" style="5" customWidth="1"/>
+    <col min="7" max="26" width="9.37890625" style="5" customWidth="1"/>
+    <col min="27" max="16384" width="12.6171875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="58.5" customHeight="1">
@@ -5531,28 +5689,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="12.9"/>
   <cols>
     <col min="1" max="1" width="8" style="16" customWidth="1"/>
     <col min="2" max="2" width="23" style="16" customWidth="1"/>
-    <col min="3" max="3" width="12.125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="43.875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="22.125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="19.125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="41.625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="41.6171875" style="16" customWidth="1"/>
     <col min="8" max="8" width="41" style="16" customWidth="1"/>
-    <col min="9" max="26" width="7.875" style="16" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="16"/>
+    <col min="9" max="26" width="7.85546875" style="16" customWidth="1"/>
+    <col min="27" max="16384" width="12.6171875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="28.5">
+    <row r="1" spans="1:26" ht="27.6">
       <c r="A1" s="50" t="s">
         <v>115</v>
       </c>
@@ -5584,7 +5742,7 @@
       <c r="Y1" s="30"/>
       <c r="Z1" s="30"/>
     </row>
-    <row r="2" spans="1:26" ht="16.5">
+    <row r="2" spans="1:26" ht="16.8">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -5610,7 +5768,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="28.5">
+    <row r="3" spans="1:26" ht="28.2">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -5632,7 +5790,7 @@
       <c r="G3" s="22"/>
       <c r="H3" s="24"/>
     </row>
-    <row r="4" spans="1:26" ht="71.25">
+    <row r="4" spans="1:26" ht="70.5">
       <c r="A4" s="20">
         <v>2</v>
       </c>
@@ -5656,7 +5814,7 @@
       </c>
       <c r="H4" s="23"/>
     </row>
-    <row r="5" spans="1:26" ht="28.5">
+    <row r="5" spans="1:26" ht="28.2">
       <c r="A5" s="20">
         <v>3</v>
       </c>
@@ -5678,7 +5836,7 @@
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
     </row>
-    <row r="6" spans="1:26" ht="42.75">
+    <row r="6" spans="1:26" ht="42.3">
       <c r="A6" s="25">
         <v>4</v>
       </c>
@@ -5700,7 +5858,7 @@
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
     </row>
-    <row r="7" spans="1:26" ht="71.25">
+    <row r="7" spans="1:26" ht="70.5">
       <c r="A7" s="25">
         <v>5</v>
       </c>
@@ -5724,7 +5882,7 @@
       </c>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" spans="1:26" ht="71.25">
+    <row r="8" spans="1:26" ht="70.5">
       <c r="A8" s="25">
         <v>6</v>
       </c>
@@ -5746,7 +5904,7 @@
       </c>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:26" ht="42.75">
+    <row r="9" spans="1:26" ht="42.3">
       <c r="A9" s="25">
         <v>7</v>
       </c>
@@ -5770,7 +5928,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25">
+    <row r="10" spans="1:26" ht="14.1">
       <c r="A10" s="25">
         <v>8</v>
       </c>
@@ -5792,7 +5950,7 @@
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
     </row>
-    <row r="11" spans="1:26" ht="57">
+    <row r="11" spans="1:26" ht="56.4">
       <c r="A11" s="25">
         <v>9</v>
       </c>
@@ -5814,7 +5972,7 @@
       <c r="G11" s="22"/>
       <c r="H11" s="27"/>
     </row>
-    <row r="12" spans="1:26" ht="14.25">
+    <row r="12" spans="1:26" ht="14.1">
       <c r="A12" s="25">
         <v>10</v>
       </c>
@@ -5836,7 +5994,7 @@
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="13" spans="1:26" ht="28.5">
+    <row r="13" spans="1:26" ht="28.2">
       <c r="A13" s="25">
         <v>11</v>
       </c>
@@ -5860,7 +6018,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="42.75">
+    <row r="14" spans="1:26" ht="42.3">
       <c r="A14" s="25">
         <v>12</v>
       </c>
@@ -5880,7 +6038,7 @@
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
     </row>
-    <row r="15" spans="1:26" ht="57">
+    <row r="15" spans="1:26" ht="56.4">
       <c r="A15" s="25">
         <v>13</v>
       </c>
@@ -5902,7 +6060,7 @@
       <c r="G15" s="22"/>
       <c r="H15" s="23"/>
     </row>
-    <row r="16" spans="1:26" ht="71.25">
+    <row r="16" spans="1:26" ht="70.5">
       <c r="A16" s="25">
         <v>14</v>
       </c>
@@ -5924,7 +6082,7 @@
       <c r="G16" s="22"/>
       <c r="H16" s="23"/>
     </row>
-    <row r="17" spans="1:8" ht="14.25">
+    <row r="17" spans="1:8" ht="14.1">
       <c r="A17" s="25">
         <v>15</v>
       </c>
@@ -5946,7 +6104,7 @@
       <c r="G17" s="22"/>
       <c r="H17" s="23"/>
     </row>
-    <row r="18" spans="1:8" ht="14.25">
+    <row r="18" spans="1:8" ht="14.1">
       <c r="A18" s="25">
         <v>16</v>
       </c>
@@ -8919,25 +9077,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="12.9"/>
   <cols>
     <col min="1" max="1" width="8" style="5" customWidth="1"/>
     <col min="2" max="2" width="23" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="43.875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="22.125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="19.125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="41.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="41.6171875" style="5" customWidth="1"/>
     <col min="8" max="8" width="41" style="5" customWidth="1"/>
-    <col min="9" max="26" width="7.875" style="5" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="5"/>
+    <col min="9" max="26" width="7.85546875" style="5" customWidth="1"/>
+    <col min="27" max="16384" width="12.6171875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="57.75" customHeight="1">
@@ -8972,7 +9130,7 @@
       <c r="Y1" s="17"/>
       <c r="Z1" s="17"/>
     </row>
-    <row r="2" spans="1:26" s="16" customFormat="1" ht="16.5">
+    <row r="2" spans="1:26" s="16" customFormat="1" ht="16.8">
       <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
@@ -8998,7 +9156,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="16" customFormat="1" ht="71.25">
+    <row r="3" spans="1:26" s="16" customFormat="1" ht="70.5">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -9024,7 +9182,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="16" customFormat="1" ht="71.25">
+    <row r="4" spans="1:26" s="16" customFormat="1" ht="70.5">
       <c r="A4" s="25">
         <v>2</v>
       </c>
@@ -9048,7 +9206,7 @@
       </c>
       <c r="H4" s="23"/>
     </row>
-    <row r="5" spans="1:26" s="16" customFormat="1" ht="28.5">
+    <row r="5" spans="1:26" s="16" customFormat="1" ht="28.2">
       <c r="A5" s="25">
         <v>3</v>
       </c>
@@ -9070,7 +9228,7 @@
       <c r="G5" s="22"/>
       <c r="H5" s="22"/>
     </row>
-    <row r="6" spans="1:26" s="16" customFormat="1" ht="42.75">
+    <row r="6" spans="1:26" s="16" customFormat="1" ht="42.3">
       <c r="A6" s="25">
         <v>4</v>
       </c>
@@ -9092,7 +9250,7 @@
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
     </row>
-    <row r="7" spans="1:26" s="16" customFormat="1" ht="14.25">
+    <row r="7" spans="1:26" s="16" customFormat="1" ht="14.1">
       <c r="A7" s="25">
         <v>5</v>
       </c>
@@ -9114,7 +9272,7 @@
       <c r="G7" s="22"/>
       <c r="H7" s="26"/>
     </row>
-    <row r="8" spans="1:26" ht="14.25">
+    <row r="8" spans="1:26" ht="14.1">
       <c r="A8" s="25">
         <v>6</v>
       </c>
@@ -9136,7 +9294,7 @@
       <c r="G8" s="22"/>
       <c r="H8" s="26"/>
     </row>
-    <row r="9" spans="1:26" ht="14.25">
+    <row r="9" spans="1:26" ht="14.1">
       <c r="A9" s="25">
         <v>7</v>
       </c>
@@ -9158,7 +9316,7 @@
       <c r="G9" s="22"/>
       <c r="H9" s="26"/>
     </row>
-    <row r="10" spans="1:26" ht="28.5">
+    <row r="10" spans="1:26" ht="28.2">
       <c r="A10" s="25">
         <v>8</v>
       </c>
@@ -9184,7 +9342,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25">
+    <row r="11" spans="1:26" ht="14.1">
       <c r="A11" s="25">
         <v>9</v>
       </c>
@@ -9206,7 +9364,7 @@
       <c r="G11" s="22"/>
       <c r="H11" s="26"/>
     </row>
-    <row r="12" spans="1:26" ht="14.25">
+    <row r="12" spans="1:26" ht="14.1">
       <c r="A12" s="25">
         <v>10</v>
       </c>
@@ -9228,7 +9386,7 @@
       <c r="G12" s="22"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:26" ht="28.5">
+    <row r="13" spans="1:26" ht="14.1">
       <c r="A13" s="25">
         <v>11</v>
       </c>
@@ -9250,7 +9408,7 @@
       <c r="G13" s="22"/>
       <c r="H13" s="26"/>
     </row>
-    <row r="14" spans="1:26" s="16" customFormat="1" ht="14.25">
+    <row r="14" spans="1:26" s="16" customFormat="1" ht="14.1">
       <c r="A14" s="25">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Modify to naracity_new xles version
</commit_message>
<xml_diff>
--- a/sample/opendata_covid19_NaraCity.xlsx
+++ b/sample/opendata_covid19_NaraCity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasushi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4837E42-F94F-4DC3-BBDE-8156705AA327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA82240-460C-49F7-B9FF-9F190EA46411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60960" yWindow="5790" windowWidth="20565" windowHeight="13890" tabRatio="775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="54075" yWindow="4935" windowWidth="23565" windowHeight="10650" tabRatio="775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.陽性患者リスト" sheetId="8" r:id="rId1"/>
@@ -19,8 +19,16 @@
     <sheet name="陽性患者リストの定義" sheetId="14" r:id="rId4"/>
     <sheet name="感染症状況の定義" sheetId="15" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId12" roundtripDataSignature="AMtx7mjH4chSrTCU+u+bcA2KRSGrmpOPZA=="/>
     </ext>
@@ -29,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="151">
   <si>
     <t>・本データ項目定義書は、新型コロナウイルス感染症対策の一環として、各自治体において標準フォーマットでのオープンデータを公開できるように支援するためのものです</t>
   </si>
@@ -1030,6 +1038,72 @@
     </rPh>
     <phoneticPr fontId="14"/>
   </si>
+  <si>
+    <t>入院有症患者数_現在</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウイン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ユウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ショウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>カンジャ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>スウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ゲンザイ</t>
+    </rPh>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>入院無症状患者数_現在</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウイン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ム</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ショウジョウ</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>カンジャスウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ゲンザイ</t>
+    </rPh>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>入院者数_累計</t>
+    <rPh sb="5" eb="7">
+      <t>ルイケイ</t>
+    </rPh>
+    <phoneticPr fontId="14"/>
+  </si>
+  <si>
+    <t>奈良市</t>
+  </si>
+  <si>
+    <t>50代</t>
+  </si>
+  <si>
+    <t>70代</t>
+  </si>
+  <si>
+    <t>無職</t>
+  </si>
+  <si>
+    <t>80代</t>
+  </si>
+  <si>
+    <t>女性</t>
+  </si>
 </sst>
 </file>
 
@@ -1040,7 +1114,7 @@
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1213,6 +1287,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1315,7 +1395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1516,6 +1596,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1735,7 +1821,7 @@
   <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2177,16 +2263,18 @@
         <v>43934</v>
       </c>
       <c r="F12" s="41"/>
-      <c r="G12" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="H12" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="I12" s="37" t="s">
-        <v>103</v>
-      </c>
-      <c r="J12" s="40"/>
+      <c r="G12" s="67" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" s="68" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="68" t="s">
+        <v>148</v>
+      </c>
       <c r="K12" s="40"/>
       <c r="L12" s="40"/>
       <c r="M12" s="40"/>
@@ -2197,39 +2285,79 @@
       <c r="P12" s="40"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="41"/>
+      <c r="A13" s="40">
+        <v>12</v>
+      </c>
+      <c r="B13" s="40">
+        <v>292010</v>
+      </c>
+      <c r="C13" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="41">
+        <v>43936</v>
+      </c>
       <c r="F13" s="41"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
+      <c r="G13" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="68" t="s">
+        <v>146</v>
+      </c>
+      <c r="I13" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="68" t="s">
+        <v>69</v>
+      </c>
       <c r="K13" s="40"/>
       <c r="L13" s="40"/>
       <c r="M13" s="40"/>
       <c r="N13" s="40"/>
-      <c r="O13" s="45"/>
+      <c r="O13" s="45">
+        <v>43936</v>
+      </c>
       <c r="P13" s="40"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="41"/>
+      <c r="A14" s="40">
+        <v>13</v>
+      </c>
+      <c r="B14" s="40">
+        <v>292010</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="41">
+        <v>43939</v>
+      </c>
       <c r="F14" s="41"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
+      <c r="G14" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="H14" s="68" t="s">
+        <v>149</v>
+      </c>
+      <c r="I14" s="68" t="s">
+        <v>150</v>
+      </c>
+      <c r="J14" s="68" t="s">
+        <v>148</v>
+      </c>
       <c r="K14" s="40"/>
       <c r="L14" s="40"/>
       <c r="M14" s="40"/>
       <c r="N14" s="40"/>
-      <c r="O14" s="45"/>
+      <c r="O14" s="45">
+        <v>43939</v>
+      </c>
       <c r="P14" s="40"/>
     </row>
     <row r="15" spans="1:16">
@@ -3195,11 +3323,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="13.8"/>
@@ -3210,14 +3338,15 @@
     <col min="4" max="4" width="12.37890625" style="35" customWidth="1"/>
     <col min="5" max="5" width="13" style="39" customWidth="1"/>
     <col min="6" max="8" width="11.37890625" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.140625" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="35" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="35" customWidth="1"/>
-    <col min="13" max="13" width="17" style="35" customWidth="1"/>
-    <col min="14" max="16384" width="8.76171875" style="35"/>
+    <col min="9" max="9" width="11.37890625" style="35" customWidth="1"/>
+    <col min="10" max="11" width="11.140625" style="35" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="11.140625" style="35" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="35" customWidth="1"/>
+    <col min="16" max="16" width="17" style="35" customWidth="1"/>
+    <col min="17" max="16384" width="8.76171875" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5">
+    <row r="1" spans="1:16" ht="31.5">
       <c r="A1" s="57" t="s">
         <v>95</v>
       </c>
@@ -3243,22 +3372,31 @@
         <v>84</v>
       </c>
       <c r="I1" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="63" t="s">
+      <c r="K1" s="63" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" s="63" t="s">
+        <v>143</v>
+      </c>
+      <c r="M1" s="63" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="N1" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="L1" s="61" t="s">
+      <c r="O1" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="M1" s="62" t="s">
+      <c r="P1" s="62" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.1">
+    <row r="2" spans="1:16" ht="14.1">
       <c r="A2" s="53">
         <v>43891</v>
       </c>
@@ -3279,15 +3417,18 @@
         <v>0</v>
       </c>
       <c r="H2" s="52"/>
-      <c r="I2" s="56"/>
+      <c r="I2" s="52"/>
       <c r="J2" s="56"/>
       <c r="K2" s="56"/>
-      <c r="L2" s="52">
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="52">
         <v>23</v>
       </c>
-      <c r="M2" s="52"/>
-    </row>
-    <row r="3" spans="1:13" ht="14.1">
+      <c r="P2" s="52"/>
+    </row>
+    <row r="3" spans="1:16" ht="14.1">
       <c r="A3" s="53">
         <v>43892</v>
       </c>
@@ -3308,15 +3449,18 @@
         <v>0</v>
       </c>
       <c r="H3" s="52"/>
-      <c r="I3" s="56"/>
+      <c r="I3" s="52"/>
       <c r="J3" s="56"/>
       <c r="K3" s="56"/>
-      <c r="L3" s="52">
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="52">
         <v>57</v>
       </c>
-      <c r="M3" s="52"/>
-    </row>
-    <row r="4" spans="1:13" ht="14.1">
+      <c r="P3" s="52"/>
+    </row>
+    <row r="4" spans="1:16" ht="14.1">
       <c r="A4" s="53">
         <v>43893</v>
       </c>
@@ -3337,15 +3481,18 @@
         <v>0</v>
       </c>
       <c r="H4" s="52"/>
-      <c r="I4" s="56"/>
+      <c r="I4" s="52"/>
       <c r="J4" s="56"/>
       <c r="K4" s="56"/>
-      <c r="L4" s="52">
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="52">
         <v>54</v>
       </c>
-      <c r="M4" s="52"/>
-    </row>
-    <row r="5" spans="1:13" ht="14.1">
+      <c r="P4" s="52"/>
+    </row>
+    <row r="5" spans="1:16" ht="14.1">
       <c r="A5" s="53">
         <v>43894</v>
       </c>
@@ -3366,15 +3513,18 @@
         <v>0</v>
       </c>
       <c r="H5" s="52"/>
-      <c r="I5" s="56"/>
+      <c r="I5" s="52"/>
       <c r="J5" s="56"/>
       <c r="K5" s="56"/>
-      <c r="L5" s="52">
+      <c r="L5" s="56"/>
+      <c r="M5" s="56"/>
+      <c r="N5" s="56"/>
+      <c r="O5" s="52">
         <v>45</v>
       </c>
-      <c r="M5" s="52"/>
-    </row>
-    <row r="6" spans="1:13" ht="14.1">
+      <c r="P5" s="52"/>
+    </row>
+    <row r="6" spans="1:16" ht="14.1">
       <c r="A6" s="53">
         <v>43895</v>
       </c>
@@ -3395,15 +3545,18 @@
         <v>0</v>
       </c>
       <c r="H6" s="52"/>
-      <c r="I6" s="56"/>
+      <c r="I6" s="52"/>
       <c r="J6" s="56"/>
       <c r="K6" s="56"/>
-      <c r="L6" s="52">
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="52">
         <v>62</v>
       </c>
-      <c r="M6" s="52"/>
-    </row>
-    <row r="7" spans="1:13" ht="14.1">
+      <c r="P6" s="52"/>
+    </row>
+    <row r="7" spans="1:16" ht="14.1">
       <c r="A7" s="53">
         <v>43896</v>
       </c>
@@ -3424,15 +3577,18 @@
         <v>3</v>
       </c>
       <c r="H7" s="52"/>
-      <c r="I7" s="56"/>
+      <c r="I7" s="52"/>
       <c r="J7" s="56"/>
       <c r="K7" s="56"/>
-      <c r="L7" s="52">
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="52">
         <v>50</v>
       </c>
-      <c r="M7" s="52"/>
-    </row>
-    <row r="8" spans="1:13" ht="14.1">
+      <c r="P7" s="52"/>
+    </row>
+    <row r="8" spans="1:16" ht="14.1">
       <c r="A8" s="53">
         <v>43897</v>
       </c>
@@ -3454,14 +3610,17 @@
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="37"/>
-      <c r="J8" s="56"/>
+      <c r="J8" s="37"/>
       <c r="K8" s="56"/>
-      <c r="L8" s="52">
+      <c r="L8" s="56"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="52">
         <v>38</v>
       </c>
-      <c r="M8" s="52"/>
-    </row>
-    <row r="9" spans="1:13" ht="14.1">
+      <c r="P8" s="52"/>
+    </row>
+    <row r="9" spans="1:16" ht="14.1">
       <c r="A9" s="53">
         <v>43898</v>
       </c>
@@ -3482,15 +3641,18 @@
         <v>0</v>
       </c>
       <c r="H9" s="52"/>
-      <c r="I9" s="56"/>
+      <c r="I9" s="52"/>
       <c r="J9" s="56"/>
       <c r="K9" s="56"/>
-      <c r="L9" s="52">
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="52">
         <v>30</v>
       </c>
-      <c r="M9" s="52"/>
-    </row>
-    <row r="10" spans="1:13" ht="14.1">
+      <c r="P9" s="52"/>
+    </row>
+    <row r="10" spans="1:16" ht="14.1">
       <c r="A10" s="53">
         <v>43899</v>
       </c>
@@ -3511,15 +3673,18 @@
         <v>0</v>
       </c>
       <c r="H10" s="52"/>
-      <c r="I10" s="56"/>
+      <c r="I10" s="52"/>
       <c r="J10" s="56"/>
       <c r="K10" s="56"/>
-      <c r="L10" s="52">
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="52">
         <v>88</v>
       </c>
-      <c r="M10" s="52"/>
-    </row>
-    <row r="11" spans="1:13" ht="14.1">
+      <c r="P10" s="52"/>
+    </row>
+    <row r="11" spans="1:16" ht="14.1">
       <c r="A11" s="53">
         <v>43900</v>
       </c>
@@ -3540,15 +3705,18 @@
         <v>0</v>
       </c>
       <c r="H11" s="52"/>
-      <c r="I11" s="56"/>
+      <c r="I11" s="52"/>
       <c r="J11" s="56"/>
       <c r="K11" s="56"/>
-      <c r="L11" s="52">
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="52">
         <v>67</v>
       </c>
-      <c r="M11" s="52"/>
-    </row>
-    <row r="12" spans="1:13" ht="14.1">
+      <c r="P11" s="52"/>
+    </row>
+    <row r="12" spans="1:16" ht="14.1">
       <c r="A12" s="53">
         <v>43901</v>
       </c>
@@ -3569,15 +3737,18 @@
         <v>1</v>
       </c>
       <c r="H12" s="52"/>
-      <c r="I12" s="56"/>
+      <c r="I12" s="52"/>
       <c r="J12" s="56"/>
       <c r="K12" s="56"/>
-      <c r="L12" s="52">
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="52">
         <v>52</v>
       </c>
-      <c r="M12" s="52"/>
-    </row>
-    <row r="13" spans="1:13" ht="14.1">
+      <c r="P12" s="52"/>
+    </row>
+    <row r="13" spans="1:16" ht="14.1">
       <c r="A13" s="53">
         <v>43902</v>
       </c>
@@ -3598,15 +3769,18 @@
         <v>0</v>
       </c>
       <c r="H13" s="52"/>
-      <c r="I13" s="56"/>
+      <c r="I13" s="52"/>
       <c r="J13" s="56"/>
       <c r="K13" s="56"/>
-      <c r="L13" s="52">
+      <c r="L13" s="56"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="52">
         <v>60</v>
       </c>
-      <c r="M13" s="52"/>
-    </row>
-    <row r="14" spans="1:13" ht="14.1">
+      <c r="P13" s="52"/>
+    </row>
+    <row r="14" spans="1:16" ht="14.1">
       <c r="A14" s="53">
         <v>43903</v>
       </c>
@@ -3627,15 +3801,18 @@
         <v>0</v>
       </c>
       <c r="H14" s="52"/>
-      <c r="I14" s="56"/>
+      <c r="I14" s="52"/>
       <c r="J14" s="56"/>
       <c r="K14" s="56"/>
-      <c r="L14" s="52">
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="52">
         <v>59</v>
       </c>
-      <c r="M14" s="52"/>
-    </row>
-    <row r="15" spans="1:13" ht="14.1">
+      <c r="P14" s="52"/>
+    </row>
+    <row r="15" spans="1:16" ht="14.1">
       <c r="A15" s="53">
         <v>43904</v>
       </c>
@@ -3656,15 +3833,18 @@
         <v>0</v>
       </c>
       <c r="H15" s="52"/>
-      <c r="I15" s="56"/>
+      <c r="I15" s="52"/>
       <c r="J15" s="56"/>
       <c r="K15" s="56"/>
-      <c r="L15" s="52">
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="52">
         <v>33</v>
       </c>
-      <c r="M15" s="52"/>
-    </row>
-    <row r="16" spans="1:13" ht="14.1">
+      <c r="P15" s="52"/>
+    </row>
+    <row r="16" spans="1:16" ht="14.1">
       <c r="A16" s="53">
         <v>43905</v>
       </c>
@@ -3685,15 +3865,18 @@
         <v>0</v>
       </c>
       <c r="H16" s="52"/>
-      <c r="I16" s="56"/>
+      <c r="I16" s="52"/>
       <c r="J16" s="56"/>
       <c r="K16" s="56"/>
-      <c r="L16" s="52">
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="52">
         <v>21</v>
       </c>
-      <c r="M16" s="52"/>
-    </row>
-    <row r="17" spans="1:13" ht="14.1">
+      <c r="P16" s="52"/>
+    </row>
+    <row r="17" spans="1:16" ht="14.1">
       <c r="A17" s="53">
         <v>43906</v>
       </c>
@@ -3714,15 +3897,18 @@
         <v>0</v>
       </c>
       <c r="H17" s="52"/>
-      <c r="I17" s="56"/>
+      <c r="I17" s="52"/>
       <c r="J17" s="56"/>
       <c r="K17" s="56"/>
-      <c r="L17" s="52">
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="52">
         <v>82</v>
       </c>
-      <c r="M17" s="52"/>
-    </row>
-    <row r="18" spans="1:13" ht="14.1">
+      <c r="P17" s="52"/>
+    </row>
+    <row r="18" spans="1:16" ht="14.1">
       <c r="A18" s="53">
         <v>43907</v>
       </c>
@@ -3743,15 +3929,18 @@
         <v>0</v>
       </c>
       <c r="H18" s="52"/>
-      <c r="I18" s="56"/>
+      <c r="I18" s="52"/>
       <c r="J18" s="56"/>
       <c r="K18" s="56"/>
-      <c r="L18" s="52">
+      <c r="L18" s="56"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="52">
         <v>34</v>
       </c>
-      <c r="M18" s="52"/>
-    </row>
-    <row r="19" spans="1:13" ht="14.1">
+      <c r="P18" s="52"/>
+    </row>
+    <row r="19" spans="1:16" ht="14.1">
       <c r="A19" s="53">
         <v>43908</v>
       </c>
@@ -3772,15 +3961,18 @@
         <v>0</v>
       </c>
       <c r="H19" s="52"/>
-      <c r="I19" s="56"/>
+      <c r="I19" s="52"/>
       <c r="J19" s="56"/>
       <c r="K19" s="56"/>
-      <c r="L19" s="52">
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="52">
         <v>60</v>
       </c>
-      <c r="M19" s="52"/>
-    </row>
-    <row r="20" spans="1:13" ht="14.1">
+      <c r="P19" s="52"/>
+    </row>
+    <row r="20" spans="1:16" ht="14.1">
       <c r="A20" s="53">
         <v>43909</v>
       </c>
@@ -3801,15 +3993,18 @@
         <v>0</v>
       </c>
       <c r="H20" s="52"/>
-      <c r="I20" s="56"/>
+      <c r="I20" s="52"/>
       <c r="J20" s="56"/>
       <c r="K20" s="56"/>
-      <c r="L20" s="52">
+      <c r="L20" s="56"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="52">
         <v>56</v>
       </c>
-      <c r="M20" s="52"/>
-    </row>
-    <row r="21" spans="1:13" ht="14.1">
+      <c r="P20" s="52"/>
+    </row>
+    <row r="21" spans="1:16" ht="14.1">
       <c r="A21" s="53">
         <v>43910</v>
       </c>
@@ -3830,15 +4025,18 @@
         <v>0</v>
       </c>
       <c r="H21" s="52"/>
-      <c r="I21" s="56"/>
+      <c r="I21" s="52"/>
       <c r="J21" s="56"/>
       <c r="K21" s="56"/>
-      <c r="L21" s="52">
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="52">
         <v>23</v>
       </c>
-      <c r="M21" s="52"/>
-    </row>
-    <row r="22" spans="1:13" ht="14.1">
+      <c r="P21" s="52"/>
+    </row>
+    <row r="22" spans="1:16" ht="14.1">
       <c r="A22" s="53">
         <v>43911</v>
       </c>
@@ -3859,15 +4057,18 @@
         <v>0</v>
       </c>
       <c r="H22" s="52"/>
-      <c r="I22" s="56"/>
+      <c r="I22" s="52"/>
       <c r="J22" s="56"/>
       <c r="K22" s="56"/>
-      <c r="L22" s="52">
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="52">
         <v>22</v>
       </c>
-      <c r="M22" s="52"/>
-    </row>
-    <row r="23" spans="1:13" ht="14.1">
+      <c r="P22" s="52"/>
+    </row>
+    <row r="23" spans="1:16" ht="14.1">
       <c r="A23" s="53">
         <v>43912</v>
       </c>
@@ -3888,15 +4089,18 @@
         <v>0</v>
       </c>
       <c r="H23" s="52"/>
-      <c r="I23" s="56"/>
+      <c r="I23" s="52"/>
       <c r="J23" s="56"/>
       <c r="K23" s="56"/>
-      <c r="L23" s="52">
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="52">
         <v>30</v>
       </c>
-      <c r="M23" s="52"/>
-    </row>
-    <row r="24" spans="1:13" ht="14.1">
+      <c r="P23" s="52"/>
+    </row>
+    <row r="24" spans="1:16" ht="14.1">
       <c r="A24" s="53">
         <v>43913</v>
       </c>
@@ -3917,15 +4121,18 @@
         <v>0</v>
       </c>
       <c r="H24" s="52"/>
-      <c r="I24" s="56"/>
+      <c r="I24" s="52"/>
       <c r="J24" s="56"/>
       <c r="K24" s="56"/>
-      <c r="L24" s="52">
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="52">
         <v>58</v>
       </c>
-      <c r="M24" s="52"/>
-    </row>
-    <row r="25" spans="1:13" ht="14.1">
+      <c r="P24" s="52"/>
+    </row>
+    <row r="25" spans="1:16" ht="14.1">
       <c r="A25" s="53">
         <v>43914</v>
       </c>
@@ -3946,15 +4153,18 @@
         <v>0</v>
       </c>
       <c r="H25" s="52"/>
-      <c r="I25" s="56"/>
+      <c r="I25" s="52"/>
       <c r="J25" s="56"/>
       <c r="K25" s="56"/>
-      <c r="L25" s="52">
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="52">
         <v>32</v>
       </c>
-      <c r="M25" s="52"/>
-    </row>
-    <row r="26" spans="1:13" ht="14.1">
+      <c r="P25" s="52"/>
+    </row>
+    <row r="26" spans="1:16" ht="14.1">
       <c r="A26" s="53">
         <v>43915</v>
       </c>
@@ -3975,15 +4185,18 @@
         <v>0</v>
       </c>
       <c r="H26" s="52"/>
-      <c r="I26" s="56"/>
+      <c r="I26" s="52"/>
       <c r="J26" s="56"/>
       <c r="K26" s="56"/>
-      <c r="L26" s="52">
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="52">
         <v>58</v>
       </c>
-      <c r="M26" s="52"/>
-    </row>
-    <row r="27" spans="1:13" ht="14.1">
+      <c r="P26" s="52"/>
+    </row>
+    <row r="27" spans="1:16" ht="14.1">
       <c r="A27" s="53">
         <v>43916</v>
       </c>
@@ -4004,15 +4217,18 @@
         <v>0</v>
       </c>
       <c r="H27" s="52"/>
-      <c r="I27" s="56"/>
+      <c r="I27" s="52"/>
       <c r="J27" s="56"/>
       <c r="K27" s="56"/>
-      <c r="L27" s="52">
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="52">
         <v>44</v>
       </c>
-      <c r="M27" s="52"/>
-    </row>
-    <row r="28" spans="1:13" ht="14.1">
+      <c r="P27" s="52"/>
+    </row>
+    <row r="28" spans="1:16" ht="14.1">
       <c r="A28" s="53">
         <v>43917</v>
       </c>
@@ -4033,15 +4249,18 @@
         <v>0</v>
       </c>
       <c r="H28" s="52"/>
-      <c r="I28" s="56"/>
+      <c r="I28" s="52"/>
       <c r="J28" s="56"/>
       <c r="K28" s="56"/>
-      <c r="L28" s="52">
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="52">
         <v>92</v>
       </c>
-      <c r="M28" s="52"/>
-    </row>
-    <row r="29" spans="1:13" ht="14.1">
+      <c r="P28" s="52"/>
+    </row>
+    <row r="29" spans="1:16" ht="14.1">
       <c r="A29" s="53">
         <v>43918</v>
       </c>
@@ -4062,15 +4281,18 @@
         <v>0</v>
       </c>
       <c r="H29" s="52"/>
-      <c r="I29" s="56"/>
+      <c r="I29" s="52"/>
       <c r="J29" s="56"/>
       <c r="K29" s="56"/>
-      <c r="L29" s="52">
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="52">
         <v>62</v>
       </c>
-      <c r="M29" s="52"/>
-    </row>
-    <row r="30" spans="1:13" ht="14.1">
+      <c r="P29" s="52"/>
+    </row>
+    <row r="30" spans="1:16" ht="14.1">
       <c r="A30" s="53">
         <v>43919</v>
       </c>
@@ -4091,15 +4313,18 @@
         <v>0</v>
       </c>
       <c r="H30" s="52"/>
-      <c r="I30" s="56"/>
+      <c r="I30" s="52"/>
       <c r="J30" s="56"/>
       <c r="K30" s="56"/>
-      <c r="L30" s="52">
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="52">
         <v>45</v>
       </c>
-      <c r="M30" s="52"/>
-    </row>
-    <row r="31" spans="1:13" ht="14.1">
+      <c r="P30" s="52"/>
+    </row>
+    <row r="31" spans="1:16" ht="14.1">
       <c r="A31" s="53">
         <v>43920</v>
       </c>
@@ -4120,15 +4345,18 @@
         <v>0</v>
       </c>
       <c r="H31" s="52"/>
-      <c r="I31" s="56"/>
+      <c r="I31" s="52"/>
       <c r="J31" s="56"/>
       <c r="K31" s="56"/>
-      <c r="L31" s="52">
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="52">
         <v>135</v>
       </c>
-      <c r="M31" s="52"/>
-    </row>
-    <row r="32" spans="1:13" ht="14.1">
+      <c r="P31" s="52"/>
+    </row>
+    <row r="32" spans="1:16" ht="14.1">
       <c r="A32" s="53">
         <v>43921</v>
       </c>
@@ -4149,15 +4377,18 @@
         <v>0</v>
       </c>
       <c r="H32" s="52"/>
-      <c r="I32" s="56"/>
+      <c r="I32" s="52"/>
       <c r="J32" s="56"/>
       <c r="K32" s="56"/>
-      <c r="L32" s="52">
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="52">
         <v>115</v>
       </c>
-      <c r="M32" s="52"/>
-    </row>
-    <row r="33" spans="1:13" ht="14.1">
+      <c r="P32" s="52"/>
+    </row>
+    <row r="33" spans="1:16" ht="14.1">
       <c r="A33" s="53">
         <v>43922</v>
       </c>
@@ -4177,12 +4408,12 @@
       <c r="G33" s="35">
         <v>1</v>
       </c>
-      <c r="L33" s="35">
+      <c r="O33" s="35">
         <v>142</v>
       </c>
-      <c r="M33" s="37"/>
-    </row>
-    <row r="34" spans="1:13" ht="14.1">
+      <c r="P33" s="37"/>
+    </row>
+    <row r="34" spans="1:16" ht="14.1">
       <c r="A34" s="53">
         <v>43923</v>
       </c>
@@ -4201,11 +4432,11 @@
       <c r="G34" s="35">
         <v>0</v>
       </c>
-      <c r="L34" s="35">
+      <c r="O34" s="35">
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="14.1">
+    <row r="35" spans="1:16" ht="14.1">
       <c r="A35" s="53">
         <v>43924</v>
       </c>
@@ -4224,11 +4455,11 @@
       <c r="G35" s="35">
         <v>0</v>
       </c>
-      <c r="L35" s="35">
+      <c r="O35" s="35">
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="14.1">
+    <row r="36" spans="1:16" ht="14.1">
       <c r="A36" s="53">
         <v>43925</v>
       </c>
@@ -4247,11 +4478,11 @@
       <c r="G36" s="35">
         <v>0</v>
       </c>
-      <c r="L36" s="35">
+      <c r="O36" s="35">
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="14.1">
+    <row r="37" spans="1:16" ht="14.1">
       <c r="A37" s="53">
         <v>43926</v>
       </c>
@@ -4270,11 +4501,11 @@
       <c r="G37" s="35">
         <v>0</v>
       </c>
-      <c r="L37" s="35">
+      <c r="O37" s="35">
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="14.1">
+    <row r="38" spans="1:16" ht="14.1">
       <c r="A38" s="53">
         <v>43927</v>
       </c>
@@ -4291,13 +4522,13 @@
         <v>4</v>
       </c>
       <c r="G38" s="35">
-        <v>1</v>
-      </c>
-      <c r="L38" s="35">
+        <v>0</v>
+      </c>
+      <c r="O38" s="35">
         <v>211</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="14.1">
+    <row r="39" spans="1:16" ht="14.1">
       <c r="A39" s="53">
         <v>43928</v>
       </c>
@@ -4314,13 +4545,13 @@
         <v>5</v>
       </c>
       <c r="G39" s="35">
-        <v>1</v>
-      </c>
-      <c r="L39" s="35">
+        <v>2</v>
+      </c>
+      <c r="O39" s="35">
         <v>142</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="14.1">
+    <row r="40" spans="1:16" ht="14.1">
       <c r="A40" s="53">
         <v>43929</v>
       </c>
@@ -4339,11 +4570,11 @@
       <c r="G40" s="66">
         <v>0</v>
       </c>
-      <c r="L40" s="35">
+      <c r="O40" s="35">
         <v>188</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="14.1">
+    <row r="41" spans="1:16" ht="14.1">
       <c r="A41" s="53">
         <v>43930</v>
       </c>
@@ -4362,11 +4593,11 @@
       <c r="G41" s="66">
         <v>2</v>
       </c>
-      <c r="L41" s="35">
+      <c r="O41" s="35">
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="14.1">
+    <row r="42" spans="1:16" ht="14.1">
       <c r="A42" s="53">
         <v>43931</v>
       </c>
@@ -4385,11 +4616,11 @@
       <c r="G42" s="66">
         <v>1</v>
       </c>
-      <c r="L42" s="35">
+      <c r="O42" s="35">
         <v>194</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="14.1">
+    <row r="43" spans="1:16" ht="14.1">
       <c r="A43" s="53">
         <v>43932</v>
       </c>
@@ -4408,11 +4639,11 @@
       <c r="G43" s="66">
         <v>0</v>
       </c>
-      <c r="L43" s="35">
+      <c r="O43" s="35">
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="14.1">
+    <row r="44" spans="1:16" ht="14.1">
       <c r="A44" s="53">
         <v>43933</v>
       </c>
@@ -4432,16 +4663,97 @@
         <v>0</v>
       </c>
       <c r="I44" s="35">
+        <v>11</v>
+      </c>
+      <c r="J44" s="35">
         <v>7</v>
       </c>
-      <c r="J44" s="35">
+      <c r="M44" s="35">
         <v>4</v>
       </c>
-      <c r="K44" s="35">
+      <c r="N44" s="35">
         <v>1</v>
       </c>
-      <c r="L44" s="35">
+      <c r="O44" s="35">
         <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="14.1">
+      <c r="A45" s="53">
+        <v>43934</v>
+      </c>
+      <c r="B45" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G45" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="14.1">
+      <c r="A46" s="53">
+        <v>43935</v>
+      </c>
+      <c r="G46" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="14.1">
+      <c r="A47" s="53">
+        <v>43936</v>
+      </c>
+      <c r="G47" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="14.1">
+      <c r="A48" s="53">
+        <v>43937</v>
+      </c>
+      <c r="G48" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="14.1">
+      <c r="A49" s="53">
+        <v>43938</v>
+      </c>
+      <c r="G49" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="14.1">
+      <c r="A50" s="53">
+        <v>43939</v>
+      </c>
+      <c r="B50" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="G50" s="66">
+        <v>1</v>
+      </c>
+      <c r="I50" s="35">
+        <v>13</v>
+      </c>
+      <c r="J50" s="35">
+        <v>9</v>
+      </c>
+      <c r="M50" s="35">
+        <v>4</v>
+      </c>
+      <c r="N50" s="35">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update naracity data sample
</commit_message>
<xml_diff>
--- a/sample/opendata_covid19_NaraCity.xlsx
+++ b/sample/opendata_covid19_NaraCity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasushi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yasushi Ishizuka\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA82240-460C-49F7-B9FF-9F190EA46411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9741D1-B20E-4E82-9936-28528EE7CAE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54075" yWindow="4935" windowWidth="23565" windowHeight="10650" tabRatio="775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52080" yWindow="-135" windowWidth="23190" windowHeight="16545" tabRatio="775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.陽性患者リスト" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="147">
   <si>
     <t>・本データ項目定義書は、新型コロナウイルス感染症対策の一環として、各自治体において標準フォーマットでのオープンデータを公開できるように支援するためのものです</t>
   </si>
@@ -1087,22 +1087,27 @@
     <phoneticPr fontId="14"/>
   </si>
   <si>
-    <t>奈良市</t>
-  </si>
-  <si>
-    <t>50代</t>
-  </si>
-  <si>
-    <t>70代</t>
-  </si>
-  <si>
-    <t>無職</t>
-  </si>
-  <si>
-    <t>80代</t>
-  </si>
-  <si>
-    <t>女性</t>
+    <t>20代</t>
+    <rPh sb="2" eb="3">
+      <t>ダイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>管外検査のためリストの１名分はカウントされず</t>
+    <rPh sb="0" eb="2">
+      <t>カンガイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ケンサ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ブン</t>
+    </rPh>
+    <phoneticPr fontId="14"/>
   </si>
 </sst>
 </file>
@@ -1114,7 +1119,7 @@
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1287,12 +1292,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1395,7 +1394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1597,11 +1596,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1821,7 +1817,7 @@
   <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A13" sqref="A13:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2263,18 +2259,16 @@
         <v>43934</v>
       </c>
       <c r="F12" s="41"/>
-      <c r="G12" s="67" t="s">
-        <v>145</v>
-      </c>
-      <c r="H12" s="68" t="s">
-        <v>147</v>
-      </c>
-      <c r="I12" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="68" t="s">
-        <v>148</v>
-      </c>
+      <c r="G12" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="I12" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="J12" s="40"/>
       <c r="K12" s="40"/>
       <c r="L12" s="40"/>
       <c r="M12" s="40"/>
@@ -2301,24 +2295,22 @@
         <v>43936</v>
       </c>
       <c r="F13" s="41"/>
-      <c r="G13" s="68" t="s">
-        <v>145</v>
-      </c>
-      <c r="H13" s="68" t="s">
-        <v>146</v>
-      </c>
-      <c r="I13" s="68" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="68" t="s">
-        <v>69</v>
-      </c>
+      <c r="G13" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>135</v>
+      </c>
+      <c r="I13" s="37" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13" s="40"/>
       <c r="K13" s="40"/>
       <c r="L13" s="40"/>
       <c r="M13" s="40"/>
       <c r="N13" s="40"/>
       <c r="O13" s="45">
-        <v>43936</v>
+        <v>43940</v>
       </c>
       <c r="P13" s="40"/>
     </row>
@@ -2339,79 +2331,131 @@
         <v>43939</v>
       </c>
       <c r="F14" s="41"/>
-      <c r="G14" s="68" t="s">
-        <v>145</v>
-      </c>
-      <c r="H14" s="68" t="s">
-        <v>149</v>
-      </c>
-      <c r="I14" s="68" t="s">
-        <v>150</v>
-      </c>
-      <c r="J14" s="68" t="s">
-        <v>148</v>
-      </c>
+      <c r="G14" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="H14" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="I14" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="J14" s="40"/>
       <c r="K14" s="40"/>
       <c r="L14" s="40"/>
       <c r="M14" s="40"/>
       <c r="N14" s="40"/>
       <c r="O14" s="45">
-        <v>43939</v>
+        <v>43940</v>
       </c>
       <c r="P14" s="40"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="41"/>
+      <c r="A15" s="40">
+        <v>14</v>
+      </c>
+      <c r="B15" s="40">
+        <v>292010</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="41">
+        <v>43942</v>
+      </c>
       <c r="F15" s="41"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
+      <c r="G15" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="H15" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="I15" s="37" t="s">
+        <v>107</v>
+      </c>
       <c r="J15" s="40"/>
       <c r="K15" s="40"/>
       <c r="L15" s="40"/>
       <c r="M15" s="40"/>
       <c r="N15" s="40"/>
-      <c r="O15" s="45"/>
+      <c r="O15" s="45">
+        <v>43948</v>
+      </c>
       <c r="P15" s="40"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="41"/>
+      <c r="A16" s="40">
+        <v>15</v>
+      </c>
+      <c r="B16" s="40">
+        <v>292010</v>
+      </c>
+      <c r="C16" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="41">
+        <v>43943</v>
+      </c>
       <c r="F16" s="41"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
+      <c r="G16" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="I16" s="37" t="s">
+        <v>103</v>
+      </c>
       <c r="J16" s="40"/>
       <c r="K16" s="40"/>
       <c r="L16" s="40"/>
       <c r="M16" s="40"/>
       <c r="N16" s="40"/>
-      <c r="O16" s="45"/>
+      <c r="O16" s="45">
+        <v>43948</v>
+      </c>
       <c r="P16" s="40"/>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="41"/>
+      <c r="A17" s="40">
+        <v>16</v>
+      </c>
+      <c r="B17" s="40">
+        <v>292010</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="41">
+        <v>43945</v>
+      </c>
       <c r="F17" s="41"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="G17" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="H17" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="I17" s="37" t="s">
+        <v>107</v>
+      </c>
       <c r="J17" s="40"/>
       <c r="K17" s="40"/>
       <c r="L17" s="40"/>
       <c r="M17" s="40"/>
       <c r="N17" s="40"/>
-      <c r="O17" s="45"/>
+      <c r="O17" s="45">
+        <v>43948</v>
+      </c>
       <c r="P17" s="40"/>
     </row>
     <row r="18" spans="1:16">
@@ -3323,11 +3367,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P50"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="13.8"/>
@@ -4522,7 +4566,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O38" s="35">
         <v>211</v>
@@ -4545,7 +4589,7 @@
         <v>5</v>
       </c>
       <c r="G39" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O39" s="35">
         <v>142</v>
@@ -4662,9 +4706,6 @@
       <c r="G44" s="66">
         <v>0</v>
       </c>
-      <c r="I44" s="35">
-        <v>11</v>
-      </c>
       <c r="J44" s="35">
         <v>7</v>
       </c>
@@ -4679,7 +4720,7 @@
       </c>
     </row>
     <row r="45" spans="1:16" ht="14.1">
-      <c r="A45" s="53">
+      <c r="A45" s="67">
         <v>43934</v>
       </c>
       <c r="B45" s="35">
@@ -4691,44 +4732,160 @@
       <c r="D45" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="G45" s="66">
+      <c r="E45" s="35"/>
+      <c r="F45" s="35">
+        <v>7</v>
+      </c>
+      <c r="G45" s="35">
+        <v>0</v>
+      </c>
+      <c r="J45" s="35">
+        <v>7</v>
+      </c>
+      <c r="M45" s="35">
+        <v>4</v>
+      </c>
+      <c r="N45" s="35">
         <v>1</v>
       </c>
+      <c r="O45" s="35">
+        <v>227</v>
+      </c>
     </row>
     <row r="46" spans="1:16" ht="14.1">
-      <c r="A46" s="53">
+      <c r="A46" s="67">
         <v>43935</v>
+      </c>
+      <c r="B46" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35">
+        <v>13</v>
       </c>
       <c r="G46" s="35">
         <v>0</v>
       </c>
+      <c r="J46" s="35">
+        <v>7</v>
+      </c>
+      <c r="M46" s="35">
+        <v>4</v>
+      </c>
+      <c r="N46" s="35">
+        <v>1</v>
+      </c>
+      <c r="O46" s="35">
+        <v>168</v>
+      </c>
     </row>
     <row r="47" spans="1:16" ht="14.1">
-      <c r="A47" s="53">
+      <c r="A47" s="67">
         <v>43936</v>
+      </c>
+      <c r="B47" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C47" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E47" s="35"/>
+      <c r="F47" s="35">
+        <v>17</v>
       </c>
       <c r="G47" s="35">
         <v>1</v>
       </c>
+      <c r="J47" s="35">
+        <v>7</v>
+      </c>
+      <c r="M47" s="35">
+        <v>5</v>
+      </c>
+      <c r="N47" s="35">
+        <v>1</v>
+      </c>
+      <c r="O47" s="35">
+        <v>162</v>
+      </c>
     </row>
     <row r="48" spans="1:16" ht="14.1">
-      <c r="A48" s="53">
+      <c r="A48" s="67">
         <v>43937</v>
+      </c>
+      <c r="B48" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35">
+        <v>24</v>
       </c>
       <c r="G48" s="35">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" ht="14.1">
-      <c r="A49" s="53">
+      <c r="J48" s="35">
+        <v>7</v>
+      </c>
+      <c r="M48" s="35">
+        <v>5</v>
+      </c>
+      <c r="N48" s="35">
+        <v>1</v>
+      </c>
+      <c r="O48" s="35">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="14.1">
+      <c r="A49" s="67">
         <v>43938</v>
       </c>
+      <c r="B49" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35">
+        <v>23</v>
+      </c>
       <c r="G49" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="14.1">
-      <c r="A50" s="53">
+        <v>1</v>
+      </c>
+      <c r="J49" s="35">
+        <v>6</v>
+      </c>
+      <c r="M49" s="35">
+        <v>6</v>
+      </c>
+      <c r="N49" s="35">
+        <v>1</v>
+      </c>
+      <c r="O49" s="35">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="14.1">
+      <c r="A50" s="67">
         <v>43939</v>
       </c>
       <c r="B50" s="35">
@@ -4740,20 +4897,285 @@
       <c r="D50" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="G50" s="66">
-        <v>1</v>
-      </c>
-      <c r="I50" s="35">
-        <v>13</v>
+      <c r="E50" s="35"/>
+      <c r="F50" s="35">
+        <v>8</v>
+      </c>
+      <c r="G50" s="35">
+        <v>0</v>
       </c>
       <c r="J50" s="35">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M50" s="35">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N50" s="35">
         <v>1</v>
+      </c>
+      <c r="O50" s="35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="14.1">
+      <c r="A51" s="67">
+        <v>43940</v>
+      </c>
+      <c r="B51" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C51" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E51" s="35"/>
+      <c r="F51" s="35">
+        <v>2</v>
+      </c>
+      <c r="G51" s="35">
+        <v>0</v>
+      </c>
+      <c r="J51" s="35">
+        <v>7</v>
+      </c>
+      <c r="M51" s="35">
+        <v>6</v>
+      </c>
+      <c r="N51" s="35">
+        <v>1</v>
+      </c>
+      <c r="O51" s="35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="14.1">
+      <c r="A52" s="67">
+        <v>43941</v>
+      </c>
+      <c r="B52" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35">
+        <v>33</v>
+      </c>
+      <c r="G52" s="35">
+        <v>0</v>
+      </c>
+      <c r="J52" s="35">
+        <v>7</v>
+      </c>
+      <c r="M52" s="35">
+        <v>6</v>
+      </c>
+      <c r="N52" s="35">
+        <v>1</v>
+      </c>
+      <c r="O52" s="35">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="14.1">
+      <c r="A53" s="67">
+        <v>43942</v>
+      </c>
+      <c r="B53" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C53" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D53" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35">
+        <v>10</v>
+      </c>
+      <c r="G53" s="35">
+        <v>2</v>
+      </c>
+      <c r="J53" s="35">
+        <v>8</v>
+      </c>
+      <c r="M53" s="35">
+        <v>6</v>
+      </c>
+      <c r="N53" s="35">
+        <v>1</v>
+      </c>
+      <c r="O53" s="35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="14.1">
+      <c r="A54" s="67">
+        <v>43943</v>
+      </c>
+      <c r="B54" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35">
+        <v>18</v>
+      </c>
+      <c r="G54" s="35">
+        <v>0</v>
+      </c>
+      <c r="J54" s="35">
+        <v>8</v>
+      </c>
+      <c r="M54" s="35">
+        <v>7</v>
+      </c>
+      <c r="N54" s="35">
+        <v>1</v>
+      </c>
+      <c r="O54" s="35">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="14.1">
+      <c r="A55" s="67">
+        <v>43944</v>
+      </c>
+      <c r="B55" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35">
+        <v>15</v>
+      </c>
+      <c r="G55" s="35">
+        <v>0</v>
+      </c>
+      <c r="J55" s="35">
+        <v>8</v>
+      </c>
+      <c r="M55" s="35">
+        <v>7</v>
+      </c>
+      <c r="N55" s="35">
+        <v>1</v>
+      </c>
+      <c r="O55" s="35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="14.1">
+      <c r="A56" s="67">
+        <v>43945</v>
+      </c>
+      <c r="B56" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C56" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D56" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35">
+        <v>29</v>
+      </c>
+      <c r="G56" s="35">
+        <v>0</v>
+      </c>
+      <c r="J56" s="35">
+        <v>9</v>
+      </c>
+      <c r="M56" s="35">
+        <v>7</v>
+      </c>
+      <c r="N56" s="35">
+        <v>1</v>
+      </c>
+      <c r="O56" s="35">
+        <v>156</v>
+      </c>
+      <c r="P56" s="37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="14.1">
+      <c r="A57" s="67">
+        <v>43946</v>
+      </c>
+      <c r="B57" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D57" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E57" s="35"/>
+      <c r="F57" s="35">
+        <v>12</v>
+      </c>
+      <c r="G57" s="35">
+        <v>0</v>
+      </c>
+      <c r="J57" s="35">
+        <v>9</v>
+      </c>
+      <c r="M57" s="35">
+        <v>7</v>
+      </c>
+      <c r="N57" s="35">
+        <v>1</v>
+      </c>
+      <c r="O57" s="35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="14.1">
+      <c r="A58" s="67">
+        <v>43947</v>
+      </c>
+      <c r="B58" s="35">
+        <v>292010</v>
+      </c>
+      <c r="C58" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D58" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E58" s="35"/>
+      <c r="J58" s="35">
+        <v>9</v>
+      </c>
+      <c r="M58" s="35">
+        <v>7</v>
+      </c>
+      <c r="N58" s="35">
+        <v>1</v>
+      </c>
+      <c r="O58" s="35">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mod convert_naracity.py, Set last date in xlsx to eachsections's date
</commit_message>
<xml_diff>
--- a/sample/opendata_covid19_NaraCity.xlsx
+++ b/sample/opendata_covid19_NaraCity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yasushi Ishizuka\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9741D1-B20E-4E82-9936-28528EE7CAE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA6038D-EDF6-4753-8878-FA14DD696DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52080" yWindow="-135" windowWidth="23190" windowHeight="16545" tabRatio="775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="73785" yWindow="8415" windowWidth="25305" windowHeight="14685" tabRatio="775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.陽性患者リスト" sheetId="8" r:id="rId1"/>
@@ -1817,7 +1817,7 @@
   <dimension ref="A1:P67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:P17"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3370,8 +3370,8 @@
   <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S40" sqref="S40"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.76171875" defaultRowHeight="13.8"/>
@@ -4704,7 +4704,7 @@
         <v>4</v>
       </c>
       <c r="G44" s="66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" s="35">
         <v>7</v>

</xml_diff>